<commit_message>
Fix connection handling and form validation
</commit_message>
<xml_diff>
--- a/Test Files/Research Product Table.xlsx
+++ b/Test Files/Research Product Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Project\WCP Research Tool WebApp\Test Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axell\WCP Project\WCP-Research-Tool-WebApp\Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4B97C7-CADF-4599-82A5-EEDECC5DD21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EFD238-2B51-46D7-BF75-33486274533C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
   <si>
     <t>Research Oem</t>
   </si>
@@ -135,6 +135,30 @@
   </si>
   <si>
     <t>Electrical</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>E2</t>
   </si>
 </sst>
 </file>
@@ -176,8 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -518,21 +541,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.09765625" customWidth="1"/>
+    <col min="7" max="7" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -554,11 +577,14 @@
       <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
         <v>101-S1-K1-U1</v>
@@ -572,22 +598,25 @@
       <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="str">
         <f>(20*10+ROW()-1)&amp;"-I"&amp;ROW()-1&amp;"-C"</f>
         <v>201-I1-C</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <f>B2&amp;" "&amp;C2&amp;" "&amp;D2</f>
         <v>Honda Sedan Sensor</v>
       </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
       <c r="H2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A5" si="0" xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
         <v>102-S2-K2-U2</v>
@@ -601,22 +630,25 @@
       <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E22" si="1">(20*10+ROW()-1)&amp;"-I"&amp;ROW()-1&amp;"-C"</f>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F22" si="1">(20*10+ROW()-1)&amp;"-I"&amp;ROW()-1&amp;"-C"</f>
         <v>202-I2-C</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F22" si="2">B3&amp;" "&amp;C3&amp;" "&amp;D3</f>
+      <c r="G3" t="str">
+        <f>B3&amp;" "&amp;C3&amp;" "&amp;D3</f>
         <v>Toyota Coupe Brakes</v>
       </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
       <c r="H3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>103-S3-K3-U3</v>
@@ -630,22 +662,25 @@
       <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="str">
         <f t="shared" si="1"/>
         <v>203-I3-C</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" si="2"/>
+      <c r="G4" t="str">
+        <f>B4&amp;" "&amp;C4&amp;" "&amp;D4</f>
         <v>Ford Convertible Suspension</v>
       </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
       <c r="H4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>104-S4-K4-U4</v>
@@ -659,22 +694,25 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="str">
         <f t="shared" si="1"/>
         <v>204-I4-C</v>
       </c>
-      <c r="F5" t="str">
-        <f t="shared" si="2"/>
+      <c r="G5" t="str">
+        <f>B5&amp;" "&amp;C5&amp;" "&amp;D5</f>
         <v>Chevrolet Hatchback Filter</v>
       </c>
-      <c r="G5" t="s">
-        <v>0</v>
-      </c>
       <c r="H5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
         <v>105-S5-K5-U5</v>
@@ -688,24 +726,27 @@
       <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="str">
         <f t="shared" si="1"/>
         <v>205-I5-C</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" si="2"/>
+      <c r="G6" t="str">
+        <f>B6&amp;" "&amp;C6&amp;" "&amp;D6</f>
         <v>Nissan SUV Engine</v>
       </c>
-      <c r="G6" t="s">
-        <v>0</v>
-      </c>
       <c r="H6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
-        <f t="shared" ref="A7:A22" si="3" xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
+        <f t="shared" ref="A7:A22" si="2" xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
         <v>106-S6-K6-U6</v>
       </c>
       <c r="B7" t="s">
@@ -717,24 +758,27 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="str">
         <f t="shared" si="1"/>
         <v>206-I6-C</v>
       </c>
-      <c r="F7" t="str">
-        <f t="shared" si="2"/>
+      <c r="G7" t="str">
+        <f>B7&amp;" "&amp;C7&amp;" "&amp;D7</f>
         <v>Volkswagen Wagon Transmission</v>
       </c>
-      <c r="G7" t="s">
-        <v>0</v>
-      </c>
       <c r="H7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>107-S7-K7-U7</v>
       </c>
       <c r="B8" t="s">
@@ -746,24 +790,27 @@
       <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="str">
         <f t="shared" si="1"/>
         <v>207-I7-C</v>
       </c>
-      <c r="F8" t="str">
-        <f t="shared" si="2"/>
+      <c r="G8" t="str">
+        <f>B8&amp;" "&amp;C8&amp;" "&amp;D8</f>
         <v>Honda Estate Electrical</v>
       </c>
-      <c r="G8" t="s">
-        <v>0</v>
-      </c>
       <c r="H8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>108-S8-K8-U8</v>
       </c>
       <c r="B9" t="s">
@@ -775,24 +822,27 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="str">
         <f t="shared" si="1"/>
         <v>208-I8-C</v>
       </c>
-      <c r="F9" t="str">
-        <f t="shared" si="2"/>
+      <c r="G9" t="str">
+        <f>B9&amp;" "&amp;C9&amp;" "&amp;D9</f>
         <v>Toyota Van Sensor</v>
       </c>
-      <c r="G9" t="s">
-        <v>0</v>
-      </c>
       <c r="H9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>109-S9-K9-U9</v>
       </c>
       <c r="B10" t="s">
@@ -804,24 +854,27 @@
       <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="str">
         <f t="shared" si="1"/>
         <v>209-I9-C</v>
       </c>
-      <c r="F10" t="str">
-        <f t="shared" si="2"/>
+      <c r="G10" t="str">
+        <f>B10&amp;" "&amp;C10&amp;" "&amp;D10</f>
         <v>Ford Pick Up Brakes</v>
       </c>
-      <c r="G10" t="s">
-        <v>0</v>
-      </c>
       <c r="H10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>110-S10-K10-U10</v>
       </c>
       <c r="B11" t="s">
@@ -833,24 +886,27 @@
       <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="str">
         <f t="shared" si="1"/>
         <v>210-I10-C</v>
       </c>
-      <c r="F11" t="str">
-        <f t="shared" si="2"/>
+      <c r="G11" t="str">
+        <f>B11&amp;" "&amp;C11&amp;" "&amp;D11</f>
         <v>Chevrolet Muscle Suspension</v>
       </c>
-      <c r="G11" t="s">
-        <v>0</v>
-      </c>
       <c r="H11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>111-S11-K11-U11</v>
       </c>
       <c r="B12" t="s">
@@ -862,24 +918,27 @@
       <c r="D12" t="s">
         <v>30</v>
       </c>
-      <c r="E12" t="str">
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="str">
         <f t="shared" si="1"/>
         <v>211-I11-C</v>
       </c>
-      <c r="F12" t="str">
-        <f t="shared" si="2"/>
+      <c r="G12" t="str">
+        <f>B12&amp;" "&amp;C12&amp;" "&amp;D12</f>
         <v>Nissan Micro Filter</v>
       </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
       <c r="H12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>112-S12-K12-U12</v>
       </c>
       <c r="B13" t="s">
@@ -891,24 +950,27 @@
       <c r="D13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" t="str">
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="str">
         <f t="shared" si="1"/>
         <v>212-I12-C</v>
       </c>
-      <c r="F13" t="str">
-        <f t="shared" si="2"/>
+      <c r="G13" t="str">
+        <f>B13&amp;" "&amp;C13&amp;" "&amp;D13</f>
         <v>Volkswagen Sedan Engine</v>
       </c>
-      <c r="G13" t="s">
-        <v>0</v>
-      </c>
       <c r="H13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>113-S13-K13-U13</v>
       </c>
       <c r="B14" t="s">
@@ -920,24 +982,27 @@
       <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="E14" t="str">
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="str">
         <f t="shared" si="1"/>
         <v>213-I13-C</v>
       </c>
-      <c r="F14" t="str">
-        <f t="shared" si="2"/>
+      <c r="G14" t="str">
+        <f>B14&amp;" "&amp;C14&amp;" "&amp;D14</f>
         <v>Honda Coupe Transmission</v>
       </c>
-      <c r="G14" t="s">
-        <v>0</v>
-      </c>
       <c r="H14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>114-S14-K14-U14</v>
       </c>
       <c r="B15" t="s">
@@ -949,24 +1014,27 @@
       <c r="D15" t="s">
         <v>33</v>
       </c>
-      <c r="E15" t="str">
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="str">
         <f t="shared" si="1"/>
         <v>214-I14-C</v>
       </c>
-      <c r="F15" t="str">
-        <f t="shared" si="2"/>
+      <c r="G15" t="str">
+        <f>B15&amp;" "&amp;C15&amp;" "&amp;D15</f>
         <v>Toyota Convertible Electrical</v>
       </c>
-      <c r="G15" t="s">
-        <v>0</v>
-      </c>
       <c r="H15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>115-S15-K15-U15</v>
       </c>
       <c r="B16" t="s">
@@ -978,24 +1046,27 @@
       <c r="D16" t="s">
         <v>27</v>
       </c>
-      <c r="E16" t="str">
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="str">
         <f t="shared" si="1"/>
         <v>215-I15-C</v>
       </c>
-      <c r="F16" t="str">
-        <f t="shared" si="2"/>
+      <c r="G16" t="str">
+        <f>B16&amp;" "&amp;C16&amp;" "&amp;D16</f>
         <v>Ford Hatchback Sensor</v>
       </c>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
       <c r="H16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>116-S16-K16-U16</v>
       </c>
       <c r="B17" t="s">
@@ -1007,24 +1078,27 @@
       <c r="D17" t="s">
         <v>28</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="str">
         <f t="shared" si="1"/>
         <v>216-I16-C</v>
       </c>
-      <c r="F17" t="str">
-        <f t="shared" si="2"/>
+      <c r="G17" t="str">
+        <f>B17&amp;" "&amp;C17&amp;" "&amp;D17</f>
         <v>Chevrolet SUV Brakes</v>
       </c>
-      <c r="G17" t="s">
-        <v>0</v>
-      </c>
       <c r="H17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>117-S17-K17-U17</v>
       </c>
       <c r="B18" t="s">
@@ -1036,24 +1110,27 @@
       <c r="D18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" t="str">
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="str">
         <f t="shared" si="1"/>
         <v>217-I17-C</v>
       </c>
-      <c r="F18" t="str">
-        <f t="shared" si="2"/>
+      <c r="G18" t="str">
+        <f>B18&amp;" "&amp;C18&amp;" "&amp;D18</f>
         <v>Nissan Wagon Suspension</v>
       </c>
-      <c r="G18" t="s">
-        <v>0</v>
-      </c>
       <c r="H18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>118-S18-K18-U18</v>
       </c>
       <c r="B19" t="s">
@@ -1065,24 +1142,27 @@
       <c r="D19" t="s">
         <v>30</v>
       </c>
-      <c r="E19" t="str">
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="str">
         <f t="shared" si="1"/>
         <v>218-I18-C</v>
       </c>
-      <c r="F19" t="str">
-        <f t="shared" si="2"/>
+      <c r="G19" t="str">
+        <f>B19&amp;" "&amp;C19&amp;" "&amp;D19</f>
         <v>Volkswagen Estate Filter</v>
       </c>
-      <c r="G19" t="s">
-        <v>0</v>
-      </c>
       <c r="H19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>119-S19-K19-U19</v>
       </c>
       <c r="B20" t="s">
@@ -1094,24 +1174,27 @@
       <c r="D20" t="s">
         <v>31</v>
       </c>
-      <c r="E20" t="str">
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="str">
         <f t="shared" si="1"/>
         <v>219-I19-C</v>
       </c>
-      <c r="F20" t="str">
-        <f t="shared" si="2"/>
+      <c r="G20" t="str">
+        <f>B20&amp;" "&amp;C20&amp;" "&amp;D20</f>
         <v>Honda Van Engine</v>
       </c>
-      <c r="G20" t="s">
-        <v>0</v>
-      </c>
       <c r="H20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>120-S20-K20-U20</v>
       </c>
       <c r="B21" t="s">
@@ -1123,24 +1206,27 @@
       <c r="D21" t="s">
         <v>32</v>
       </c>
-      <c r="E21" t="str">
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" t="str">
         <f t="shared" si="1"/>
         <v>220-I20-C</v>
       </c>
-      <c r="F21" t="str">
-        <f t="shared" si="2"/>
+      <c r="G21" t="str">
+        <f>B21&amp;" "&amp;C21&amp;" "&amp;D21</f>
         <v>Toyota Pick Up Transmission</v>
       </c>
-      <c r="G21" t="s">
-        <v>0</v>
-      </c>
       <c r="H21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>121-S21-K21-U21</v>
       </c>
       <c r="B22" t="s">
@@ -1152,25 +1238,25 @@
       <c r="D22" t="s">
         <v>33</v>
       </c>
-      <c r="E22" t="str">
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="str">
         <f t="shared" si="1"/>
         <v>221-I21-C</v>
       </c>
-      <c r="F22" t="str">
-        <f t="shared" si="2"/>
+      <c r="G22" t="str">
+        <f>B22&amp;" "&amp;C22&amp;" "&amp;D22</f>
         <v>Ford Muscle Electrical</v>
       </c>
-      <c r="G22" t="s">
-        <v>0</v>
-      </c>
       <c r="H22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H1"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implement TODOs and make code improvements
</commit_message>
<xml_diff>
--- a/Test Files/Research Product Table.xlsx
+++ b/Test Files/Research Product Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axell\WCP Project\WCP-Research-Tool-WebApp\Test Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Project\WCP Research Tool WebApp\Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EFD238-2B51-46D7-BF75-33486274533C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8F0A60-CE84-49FF-B452-FDB25736A36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7095" yWindow="660" windowWidth="13230" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -543,19 +543,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" customWidth="1"/>
-    <col min="7" max="7" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="7" max="7" width="17.75" customWidth="1"/>
+    <col min="8" max="8" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -584,7 +583,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
         <v>101-S1-K1-U1</v>
@@ -596,17 +595,17 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
       </c>
       <c r="F2" t="str">
         <f>(20*10+ROW()-1)&amp;"-I"&amp;ROW()-1&amp;"-C"</f>
         <v>201-I1-C</v>
       </c>
       <c r="G2" t="str">
-        <f>B2&amp;" "&amp;C2&amp;" "&amp;D2</f>
+        <f t="shared" ref="G2:G22" si="0">B2&amp;" "&amp;C2&amp;" "&amp;E2</f>
         <v>Honda Sedan Sensor</v>
       </c>
       <c r="H2" t="s">
@@ -616,9 +615,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A5" si="0" xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
+        <f t="shared" ref="A3:A5" si="1" xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
         <v>102-S2-K2-U2</v>
       </c>
       <c r="B3" t="s">
@@ -628,17 +627,17 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F22" si="1">(20*10+ROW()-1)&amp;"-I"&amp;ROW()-1&amp;"-C"</f>
+        <f t="shared" ref="F3:F22" si="2">(20*10+ROW()-1)&amp;"-I"&amp;ROW()-1&amp;"-C"</f>
         <v>202-I2-C</v>
       </c>
       <c r="G3" t="str">
-        <f>B3&amp;" "&amp;C3&amp;" "&amp;D3</f>
+        <f t="shared" si="0"/>
         <v>Toyota Coupe Brakes</v>
       </c>
       <c r="H3" t="s">
@@ -648,9 +647,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>103-S3-K3-U3</v>
       </c>
       <c r="B4" t="s">
@@ -660,29 +659,29 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
       <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>203-I3-C</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>Ford Convertible Suspension</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
         <f t="shared" si="1"/>
-        <v>203-I3-C</v>
-      </c>
-      <c r="G4" t="str">
-        <f>B4&amp;" "&amp;C4&amp;" "&amp;D4</f>
-        <v>Ford Convertible Suspension</v>
-      </c>
-      <c r="H4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f t="shared" si="0"/>
         <v>104-S4-K4-U4</v>
       </c>
       <c r="B5" t="s">
@@ -692,17 +691,17 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
       <c r="F5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>204-I4-C</v>
       </c>
       <c r="G5" t="str">
-        <f>B5&amp;" "&amp;C5&amp;" "&amp;D5</f>
+        <f t="shared" si="0"/>
         <v>Chevrolet Hatchback Filter</v>
       </c>
       <c r="H5" t="s">
@@ -712,7 +711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
         <v>105-S5-K5-U5</v>
@@ -724,17 +723,17 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
       <c r="F6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>205-I5-C</v>
       </c>
       <c r="G6" t="str">
-        <f>B6&amp;" "&amp;C6&amp;" "&amp;D6</f>
+        <f t="shared" si="0"/>
         <v>Nissan SUV Engine</v>
       </c>
       <c r="H6" t="s">
@@ -744,9 +743,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f t="shared" ref="A7:A22" si="2" xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
+        <f t="shared" ref="A7:A22" si="3" xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
         <v>106-S6-K6-U6</v>
       </c>
       <c r="B7" t="s">
@@ -756,17 +755,17 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
       <c r="F7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>206-I6-C</v>
       </c>
       <c r="G7" t="str">
-        <f>B7&amp;" "&amp;C7&amp;" "&amp;D7</f>
+        <f t="shared" si="0"/>
         <v>Volkswagen Wagon Transmission</v>
       </c>
       <c r="H7" t="s">
@@ -776,9 +775,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>107-S7-K7-U7</v>
       </c>
       <c r="B8" t="s">
@@ -788,17 +787,17 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
       <c r="F8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>207-I7-C</v>
       </c>
       <c r="G8" t="str">
-        <f>B8&amp;" "&amp;C8&amp;" "&amp;D8</f>
+        <f t="shared" si="0"/>
         <v>Honda Estate Electrical</v>
       </c>
       <c r="H8" t="s">
@@ -808,9 +807,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108-S8-K8-U8</v>
       </c>
       <c r="B9" t="s">
@@ -820,17 +819,17 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
       <c r="F9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>208-I8-C</v>
       </c>
       <c r="G9" t="str">
-        <f>B9&amp;" "&amp;C9&amp;" "&amp;D9</f>
+        <f t="shared" si="0"/>
         <v>Toyota Van Sensor</v>
       </c>
       <c r="H9" t="s">
@@ -840,9 +839,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109-S9-K9-U9</v>
       </c>
       <c r="B10" t="s">
@@ -852,17 +851,17 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
       <c r="F10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>209-I9-C</v>
       </c>
       <c r="G10" t="str">
-        <f>B10&amp;" "&amp;C10&amp;" "&amp;D10</f>
+        <f t="shared" si="0"/>
         <v>Ford Pick Up Brakes</v>
       </c>
       <c r="H10" t="s">
@@ -872,9 +871,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110-S10-K10-U10</v>
       </c>
       <c r="B11" t="s">
@@ -884,17 +883,17 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
       <c r="F11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>210-I10-C</v>
       </c>
       <c r="G11" t="str">
-        <f>B11&amp;" "&amp;C11&amp;" "&amp;D11</f>
+        <f t="shared" si="0"/>
         <v>Chevrolet Muscle Suspension</v>
       </c>
       <c r="H11" t="s">
@@ -904,9 +903,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111-S11-K11-U11</v>
       </c>
       <c r="B12" t="s">
@@ -916,17 +915,17 @@
         <v>26</v>
       </c>
       <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
         <v>30</v>
       </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
       <c r="F12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>211-I11-C</v>
       </c>
       <c r="G12" t="str">
-        <f>B12&amp;" "&amp;C12&amp;" "&amp;D12</f>
+        <f t="shared" si="0"/>
         <v>Nissan Micro Filter</v>
       </c>
       <c r="H12" t="s">
@@ -936,9 +935,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>112-S12-K12-U12</v>
       </c>
       <c r="B13" t="s">
@@ -948,17 +947,17 @@
         <v>16</v>
       </c>
       <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" t="s">
-        <v>39</v>
-      </c>
       <c r="F13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>212-I12-C</v>
       </c>
       <c r="G13" t="str">
-        <f>B13&amp;" "&amp;C13&amp;" "&amp;D13</f>
+        <f t="shared" si="0"/>
         <v>Volkswagen Sedan Engine</v>
       </c>
       <c r="H13" t="s">
@@ -968,9 +967,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113-S13-K13-U13</v>
       </c>
       <c r="B14" t="s">
@@ -980,17 +979,17 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
         <v>32</v>
       </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
       <c r="F14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>213-I13-C</v>
       </c>
       <c r="G14" t="str">
-        <f>B14&amp;" "&amp;C14&amp;" "&amp;D14</f>
+        <f t="shared" si="0"/>
         <v>Honda Coupe Transmission</v>
       </c>
       <c r="H14" t="s">
@@ -1000,9 +999,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114-S14-K14-U14</v>
       </c>
       <c r="B15" t="s">
@@ -1012,17 +1011,17 @@
         <v>18</v>
       </c>
       <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="E15" t="s">
-        <v>41</v>
-      </c>
       <c r="F15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>214-I14-C</v>
       </c>
       <c r="G15" t="str">
-        <f>B15&amp;" "&amp;C15&amp;" "&amp;D15</f>
+        <f t="shared" si="0"/>
         <v>Toyota Convertible Electrical</v>
       </c>
       <c r="H15" t="s">
@@ -1032,9 +1031,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115-S15-K15-U15</v>
       </c>
       <c r="B16" t="s">
@@ -1044,17 +1043,17 @@
         <v>19</v>
       </c>
       <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
         <v>27</v>
       </c>
-      <c r="E16" t="s">
-        <v>35</v>
-      </c>
       <c r="F16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>215-I15-C</v>
       </c>
       <c r="G16" t="str">
-        <f>B16&amp;" "&amp;C16&amp;" "&amp;D16</f>
+        <f t="shared" si="0"/>
         <v>Ford Hatchback Sensor</v>
       </c>
       <c r="H16" t="s">
@@ -1064,9 +1063,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>116-S16-K16-U16</v>
       </c>
       <c r="B17" t="s">
@@ -1076,17 +1075,17 @@
         <v>20</v>
       </c>
       <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
         <v>28</v>
       </c>
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
       <c r="F17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>216-I16-C</v>
       </c>
       <c r="G17" t="str">
-        <f>B17&amp;" "&amp;C17&amp;" "&amp;D17</f>
+        <f t="shared" si="0"/>
         <v>Chevrolet SUV Brakes</v>
       </c>
       <c r="H17" t="s">
@@ -1096,9 +1095,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117-S17-K17-U17</v>
       </c>
       <c r="B18" t="s">
@@ -1108,17 +1107,17 @@
         <v>21</v>
       </c>
       <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" t="s">
-        <v>36</v>
-      </c>
       <c r="F18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>217-I17-C</v>
       </c>
       <c r="G18" t="str">
-        <f>B18&amp;" "&amp;C18&amp;" "&amp;D18</f>
+        <f t="shared" si="0"/>
         <v>Nissan Wagon Suspension</v>
       </c>
       <c r="H18" t="s">
@@ -1128,9 +1127,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>118-S18-K18-U18</v>
       </c>
       <c r="B19" t="s">
@@ -1140,17 +1139,17 @@
         <v>22</v>
       </c>
       <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
         <v>30</v>
       </c>
-      <c r="E19" t="s">
-        <v>38</v>
-      </c>
       <c r="F19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>218-I18-C</v>
       </c>
       <c r="G19" t="str">
-        <f>B19&amp;" "&amp;C19&amp;" "&amp;D19</f>
+        <f t="shared" si="0"/>
         <v>Volkswagen Estate Filter</v>
       </c>
       <c r="H19" t="s">
@@ -1160,9 +1159,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>119-S19-K19-U19</v>
       </c>
       <c r="B20" t="s">
@@ -1172,17 +1171,17 @@
         <v>23</v>
       </c>
       <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
         <v>31</v>
       </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
       <c r="F20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>219-I19-C</v>
       </c>
       <c r="G20" t="str">
-        <f>B20&amp;" "&amp;C20&amp;" "&amp;D20</f>
+        <f t="shared" si="0"/>
         <v>Honda Van Engine</v>
       </c>
       <c r="H20" t="s">
@@ -1192,9 +1191,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120-S20-K20-U20</v>
       </c>
       <c r="B21" t="s">
@@ -1204,17 +1203,17 @@
         <v>24</v>
       </c>
       <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
         <v>32</v>
       </c>
-      <c r="E21" t="s">
-        <v>40</v>
-      </c>
       <c r="F21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>220-I20-C</v>
       </c>
       <c r="G21" t="str">
-        <f>B21&amp;" "&amp;C21&amp;" "&amp;D21</f>
+        <f t="shared" si="0"/>
         <v>Toyota Pick Up Transmission</v>
       </c>
       <c r="H21" t="s">
@@ -1224,9 +1223,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121-S21-K21-U21</v>
       </c>
       <c r="B22" t="s">
@@ -1236,17 +1235,17 @@
         <v>25</v>
       </c>
       <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
         <v>33</v>
       </c>
-      <c r="E22" t="s">
-        <v>41</v>
-      </c>
       <c r="F22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>221-I21-C</v>
       </c>
       <c r="G22" t="str">
-        <f>B22&amp;" "&amp;C22&amp;" "&amp;D22</f>
+        <f t="shared" si="0"/>
         <v>Ford Muscle Electrical</v>
       </c>
       <c r="H22" t="s">

</xml_diff>

<commit_message>
Update SQL queries and import functionality
</commit_message>
<xml_diff>
--- a/Test Files/Research Product Table.xlsx
+++ b/Test Files/Research Product Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Project\WCP Research Tool WebApp\Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8F0A60-CE84-49FF-B452-FDB25736A36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239EEDC6-4ED0-4B44-BF02-272DF63A4F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="660" windowWidth="13230" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5565" yWindow="4860" windowWidth="17580" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="57">
   <si>
     <t>Research Oem</t>
   </si>
   <si>
-    <t>Aftermarket</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -119,24 +116,6 @@
     <t>Sensor</t>
   </si>
   <si>
-    <t>Brakes</t>
-  </si>
-  <si>
-    <t>Suspension</t>
-  </si>
-  <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>Engine</t>
-  </si>
-  <si>
-    <t>Transmission</t>
-  </si>
-  <si>
-    <t>Electrical</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
@@ -159,6 +138,72 @@
   </si>
   <si>
     <t>E2</t>
+  </si>
+  <si>
+    <t>Sensor1</t>
+  </si>
+  <si>
+    <t>Brakes1</t>
+  </si>
+  <si>
+    <t>Suspension1</t>
+  </si>
+  <si>
+    <t>Filter1</t>
+  </si>
+  <si>
+    <t>Engine1</t>
+  </si>
+  <si>
+    <t>Transmission1</t>
+  </si>
+  <si>
+    <t>Electrical1</t>
+  </si>
+  <si>
+    <t>Sensor2</t>
+  </si>
+  <si>
+    <t>Brakes2</t>
+  </si>
+  <si>
+    <t>Suspension2</t>
+  </si>
+  <si>
+    <t>Filter2</t>
+  </si>
+  <si>
+    <t>Engine2</t>
+  </si>
+  <si>
+    <t>Transmission2</t>
+  </si>
+  <si>
+    <t>Electrical2</t>
+  </si>
+  <si>
+    <t>Sensor3</t>
+  </si>
+  <si>
+    <t>Brakes3</t>
+  </si>
+  <si>
+    <t>Suspension3</t>
+  </si>
+  <si>
+    <t>Filter3</t>
+  </si>
+  <si>
+    <t>Engine3</t>
+  </si>
+  <si>
+    <t>Transmission3</t>
+  </si>
+  <si>
+    <t>Electrical3</t>
+  </si>
+  <si>
+    <t>Genuine</t>
   </si>
 </sst>
 </file>
@@ -541,9 +586,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -556,31 +603,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -589,16 +636,16 @@
         <v>101-S1-K1-U1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
         <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
       </c>
       <c r="F2" t="str">
         <f>(20*10+ROW()-1)&amp;"-I"&amp;ROW()-1&amp;"-C"</f>
@@ -606,13 +653,13 @@
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G22" si="0">B2&amp;" "&amp;C2&amp;" "&amp;E2</f>
-        <v>Honda Sedan Sensor</v>
+        <v>Honda Sedan Sensor1</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -621,16 +668,16 @@
         <v>102-S2-K2-U2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F22" si="2">(20*10+ROW()-1)&amp;"-I"&amp;ROW()-1&amp;"-C"</f>
@@ -638,13 +685,13 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>Toyota Coupe Brakes</v>
+        <v>Toyota Coupe Brakes1</v>
       </c>
       <c r="H3" t="s">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -653,16 +700,16 @@
         <v>103-S3-K3-U3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
@@ -670,13 +717,13 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>Ford Convertible Suspension</v>
+        <v>Ford Convertible Suspension1</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -685,30 +732,30 @@
         <v>104-S4-K4-U4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
         <v>38</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
         <v>204-I4-C</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>Chevrolet Hatchback Filter</v>
+        <v>Chevrolet Hatchback Filter1</v>
       </c>
       <c r="H5" t="s">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -717,30 +764,30 @@
         <v>105-S5-K5-U5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
         <v>39</v>
       </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
         <v>205-I5-C</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>Nissan SUV Engine</v>
+        <v>Nissan SUV Engine1</v>
       </c>
       <c r="H6" t="s">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -749,30 +796,30 @@
         <v>106-S6-K6-U6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
         <v>40</v>
       </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
         <v>206-I6-C</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>Volkswagen Wagon Transmission</v>
+        <v>Volkswagen Wagon Transmission1</v>
       </c>
       <c r="H7" t="s">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -781,30 +828,30 @@
         <v>107-S7-K7-U7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
         <v>207-I7-C</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>Honda Estate Electrical</v>
+        <v>Honda Estate Electrical1</v>
       </c>
       <c r="H8" t="s">
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -813,16 +860,16 @@
         <v>108-S8-K8-U8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
@@ -830,13 +877,13 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>Toyota Van Sensor</v>
+        <v>Toyota Van Sensor2</v>
       </c>
       <c r="H9" t="s">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -845,16 +892,16 @@
         <v>109-S9-K9-U9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
@@ -862,13 +909,13 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>Ford Pick Up Brakes</v>
+        <v>Ford Pick Up Brakes2</v>
       </c>
       <c r="H10" t="s">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -877,16 +924,16 @@
         <v>110-S10-K10-U10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
@@ -894,13 +941,13 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>Chevrolet Muscle Suspension</v>
+        <v>Chevrolet Muscle Suspension2</v>
       </c>
       <c r="H11" t="s">
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -909,16 +956,16 @@
         <v>111-S11-K11-U11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
@@ -926,13 +973,13 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>Nissan Micro Filter</v>
+        <v>Nissan Micro Filter2</v>
       </c>
       <c r="H12" t="s">
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -941,16 +988,16 @@
         <v>112-S12-K12-U12</v>
       </c>
       <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
@@ -958,13 +1005,13 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>Volkswagen Sedan Engine</v>
+        <v>Volkswagen Sedan Engine2</v>
       </c>
       <c r="H13" t="s">
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -973,16 +1020,16 @@
         <v>113-S13-K13-U13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
@@ -990,13 +1037,13 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>Honda Coupe Transmission</v>
+        <v>Honda Coupe Transmission2</v>
       </c>
       <c r="H14" t="s">
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1005,16 +1052,16 @@
         <v>114-S14-K14-U14</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
@@ -1022,13 +1069,13 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>Toyota Convertible Electrical</v>
+        <v>Toyota Convertible Electrical2</v>
       </c>
       <c r="H15" t="s">
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1037,16 +1084,16 @@
         <v>115-S15-K15-U15</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
@@ -1054,13 +1101,13 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>Ford Hatchback Sensor</v>
+        <v>Ford Hatchback Sensor3</v>
       </c>
       <c r="H16" t="s">
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1069,16 +1116,16 @@
         <v>116-S16-K16-U16</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="2"/>
@@ -1086,13 +1133,13 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>Chevrolet SUV Brakes</v>
+        <v>Chevrolet SUV Brakes3</v>
       </c>
       <c r="H17" t="s">
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1101,16 +1148,16 @@
         <v>117-S17-K17-U17</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
@@ -1118,13 +1165,13 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>Nissan Wagon Suspension</v>
+        <v>Nissan Wagon Suspension3</v>
       </c>
       <c r="H18" t="s">
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1133,16 +1180,16 @@
         <v>118-S18-K18-U18</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="2"/>
@@ -1150,13 +1197,13 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>Volkswagen Estate Filter</v>
+        <v>Volkswagen Estate Filter3</v>
       </c>
       <c r="H19" t="s">
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1165,16 +1212,16 @@
         <v>119-S19-K19-U19</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="2"/>
@@ -1182,13 +1229,13 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>Honda Van Engine</v>
+        <v>Honda Van Engine3</v>
       </c>
       <c r="H20" t="s">
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1197,16 +1244,16 @@
         <v>120-S20-K20-U20</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="2"/>
@@ -1214,13 +1261,13 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>Toyota Pick Up Transmission</v>
+        <v>Toyota Pick Up Transmission3</v>
       </c>
       <c r="H21" t="s">
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1229,16 +1276,16 @@
         <v>121-S21-K21-U21</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="2"/>
@@ -1246,13 +1293,45 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>Ford Muscle Electrical</v>
+        <v>Ford Muscle Electrical3</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>1</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f xml:space="preserve"> (10*10+ROW()-1)&amp;"-S"&amp;ROW()-1&amp;"-K"&amp;ROW()-1&amp;"-U"&amp;ROW()-1</f>
+        <v>122-S22-K22-U22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="str">
+        <f>(20*10+ROW()-1)&amp;"-I"&amp;ROW()-1&amp;"-C"</f>
+        <v>222-I22-C</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" ref="G23" si="4">B23&amp;" "&amp;C23&amp;" "&amp;E23</f>
+        <v>Honda Sedan Sensor</v>
+      </c>
+      <c r="H23" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SQL queries and add optional supplier number parameter
</commit_message>
<xml_diff>
--- a/Test Files/Research Product Table.xlsx
+++ b/Test Files/Research Product Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Project\WCP Research Tool WebApp\Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239EEDC6-4ED0-4B44-BF02-272DF63A4F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40F8AB9-76C5-4ADA-94A8-58E2EFF08F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5565" yWindow="4860" windowWidth="17580" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="58">
   <si>
     <t>Research Oem</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Genuine</t>
+  </si>
+  <si>
+    <t>Aftermarket</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -659,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -691,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -723,7 +726,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -755,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -787,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -819,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -851,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -883,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -915,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>